<commit_message>
Fix bug in templates.xlsx
- fix broken mro-serotype-molecules.csv
- update MRO_UNSTABLE.owl with serotype molecules
</commit_message>
<xml_diff>
--- a/src/mro/templates.xlsx
+++ b/src/mro/templates.xlsx
@@ -195,9 +195,6 @@
     <t>$prefix molecule with $haplotype haplotype</t>
   </si>
   <si>
-    <t>serotype-molecule</t>
-  </si>
-  <si>
     <t>$class molecule with serotype</t>
   </si>
   <si>
@@ -223,6 +220,9 @@
   </si>
   <si>
     <t>Mutant Of</t>
+  </si>
+  <si>
+    <t>serotype-molecules</t>
   </si>
 </sst>
 </file>
@@ -727,7 +727,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E33" sqref="E33"/>
+      <selection pane="bottomLeft" activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -779,7 +779,7 @@
         <v>53</v>
       </c>
       <c r="M1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:13">
@@ -1357,13 +1357,13 @@
     </row>
     <row r="28" spans="1:12">
       <c r="A28" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="B28">
         <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E28" t="s">
         <v>18</v>
@@ -1377,13 +1377,13 @@
     </row>
     <row r="29" spans="1:12">
       <c r="A29" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="B29">
         <v>2</v>
       </c>
       <c r="C29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E29" t="s">
         <v>18</v>
@@ -1401,13 +1401,13 @@
     </row>
     <row r="30" spans="1:12">
       <c r="A30" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="B30">
         <v>3</v>
       </c>
       <c r="C30" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E30" t="s">
         <v>18</v>
@@ -1425,30 +1425,30 @@
     </row>
     <row r="31" spans="1:12">
       <c r="A31" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B31">
         <v>1</v>
       </c>
       <c r="C31" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E31" t="s">
         <v>8</v>
       </c>
       <c r="F31" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="32" spans="1:12">
       <c r="A32" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B32">
         <v>2</v>
       </c>
       <c r="C32" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E32" t="s">
         <v>8</v>
@@ -1460,13 +1460,13 @@
     </row>
     <row r="33" spans="1:13">
       <c r="A33" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B33">
         <v>3</v>
       </c>
       <c r="C33" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E33" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
Fix templates again for serotype-molecules
</commit_message>
<xml_diff>
--- a/src/mro/templates.xlsx
+++ b/src/mro/templates.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25915"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="40" yWindow="0" windowWidth="17240" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="800" yWindow="0" windowWidth="17240" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="68">
   <si>
     <t>Branch</t>
   </si>
@@ -725,9 +725,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A31" sqref="A31"/>
+      <selection pane="bottomLeft" activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1371,8 +1371,9 @@
       <c r="F28" t="s">
         <v>55</v>
       </c>
-      <c r="L28" t="s">
-        <v>26</v>
+      <c r="L28" t="str">
+        <f>C9</f>
+        <v>$class serotype</v>
       </c>
     </row>
     <row r="29" spans="1:12">

</xml_diff>

<commit_message>
Update with GO and SO terms
- use GO:0042611 'MHC protein complex'
- use SO:0001024 'haplotype' and SO:0000355 'haplotype_block'
- use "protein complex" instead of "molecule" throughout
</commit_message>
<xml_diff>
--- a/src/mro/templates.xlsx
+++ b/src/mro/templates.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25915"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="40" yWindow="0" windowWidth="17240" windowHeight="15540" tabRatio="500"/>
@@ -135,18 +135,6 @@
     <t>molecules</t>
   </si>
   <si>
-    <t>$class molecule</t>
-  </si>
-  <si>
-    <t>MHC molecule</t>
-  </si>
-  <si>
-    <t>$taxon-label $class molecule</t>
-  </si>
-  <si>
-    <t>$prefix-$locus molecule</t>
-  </si>
-  <si>
     <t>Alpha Chain</t>
   </si>
   <si>
@@ -159,12 +147,6 @@
     <t>Beta-2-microglobulin chain</t>
   </si>
   <si>
-    <t>$prefix-$chain-ii-locus molecule</t>
-  </si>
-  <si>
-    <t>$molecule molecule</t>
-  </si>
-  <si>
     <t>With Haplotype</t>
   </si>
   <si>
@@ -177,36 +159,12 @@
     <t>protein complex</t>
   </si>
   <si>
-    <t>$taxon-label MHC molecule with haplotype</t>
-  </si>
-  <si>
-    <t>$prefix molecule with $haplotype haplotype</t>
-  </si>
-  <si>
-    <t>$class molecule with serotype</t>
-  </si>
-  <si>
-    <t>$taxon-label $class molecule with serotype</t>
-  </si>
-  <si>
-    <t>$prefix molecule with $serotype serotype</t>
-  </si>
-  <si>
     <t>mutant-molecules</t>
   </si>
   <si>
-    <t>mutant $class molecule</t>
-  </si>
-  <si>
-    <t>mutant $taxon-label $class molecule</t>
-  </si>
-  <si>
     <t>$label</t>
   </si>
   <si>
-    <t>mutant MHC molecule</t>
-  </si>
-  <si>
     <t>Mutant Of</t>
   </si>
   <si>
@@ -274,6 +232,48 @@
   </si>
   <si>
     <t>class II not sublocus?</t>
+  </si>
+  <si>
+    <t>MHC protein complex</t>
+  </si>
+  <si>
+    <t>mutant MHC protein complex</t>
+  </si>
+  <si>
+    <t>$taxon-label $class protein complex</t>
+  </si>
+  <si>
+    <t>$prefix-$locus protein complex</t>
+  </si>
+  <si>
+    <t>$prefix-$chain-ii-locus protein complex</t>
+  </si>
+  <si>
+    <t>$taxon-label MHC protein complex with haplotype</t>
+  </si>
+  <si>
+    <t>$prefix protein complex with $haplotype haplotype</t>
+  </si>
+  <si>
+    <t>$class protein complex with serotype</t>
+  </si>
+  <si>
+    <t>$taxon-label $class protein complex with serotype</t>
+  </si>
+  <si>
+    <t>$prefix protein complex with $serotype serotype</t>
+  </si>
+  <si>
+    <t>mutant $class protein complex</t>
+  </si>
+  <si>
+    <t>mutant $taxon-label $class protein complex</t>
+  </si>
+  <si>
+    <t>$class protein complex</t>
+  </si>
+  <si>
+    <t>$molecule protein complex</t>
   </si>
 </sst>
 </file>
@@ -832,16 +832,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F24" sqref="F24"/>
+      <selection pane="bottomLeft" activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31" customWidth="1"/>
     <col min="4" max="4" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.5" customWidth="1"/>
     <col min="6" max="6" width="14.5" customWidth="1"/>
@@ -861,7 +861,7 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="E1" t="s">
         <v>13</v>
@@ -882,19 +882,19 @@
         <v>4</v>
       </c>
       <c r="K1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L1" t="s">
+        <v>39</v>
+      </c>
+      <c r="M1" t="s">
         <v>42</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>43</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>48</v>
-      </c>
-      <c r="N1" t="s">
-        <v>49</v>
-      </c>
-      <c r="O1" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:15">
@@ -946,7 +946,7 @@
         <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="G4" t="s">
         <v>8</v>
@@ -967,7 +967,7 @@
         <v>15</v>
       </c>
       <c r="F5" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="G5" t="s">
         <v>8</v>
@@ -988,13 +988,13 @@
         <v>12</v>
       </c>
       <c r="F6" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="G6" t="s">
         <v>8</v>
       </c>
       <c r="H6" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:15">
@@ -1008,13 +1008,13 @@
         <v>15</v>
       </c>
       <c r="F7" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="G7" t="s">
         <v>8</v>
       </c>
       <c r="H7" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:15">
@@ -1251,7 +1251,7 @@
         <v>35</v>
       </c>
       <c r="F19" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="G19" t="s">
         <v>8</v>
@@ -1272,7 +1272,7 @@
         <v>36</v>
       </c>
       <c r="F20" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="G20" t="s">
         <v>8</v>
@@ -1290,19 +1290,19 @@
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>38</v>
+        <v>83</v>
       </c>
       <c r="D21" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="E21" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="G21" t="s">
         <v>8</v>
       </c>
       <c r="H21" t="s">
-        <v>39</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" spans="1:14">
@@ -1313,7 +1313,7 @@
         <v>2</v>
       </c>
       <c r="C22" t="s">
-        <v>40</v>
+        <v>73</v>
       </c>
       <c r="D22" t="s">
         <v>11</v>
@@ -1323,7 +1323,7 @@
       </c>
       <c r="H22" t="str">
         <f>C21</f>
-        <v>$class molecule</v>
+        <v>$class protein complex</v>
       </c>
       <c r="I22" t="s">
         <v>11</v>
@@ -1337,23 +1337,23 @@
         <v>3</v>
       </c>
       <c r="C23" t="s">
-        <v>41</v>
+        <v>74</v>
       </c>
       <c r="D23" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="E23" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="F23" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="G23" t="s">
         <v>18</v>
       </c>
       <c r="H23" t="str">
         <f>C21</f>
-        <v>$class molecule</v>
+        <v>$class protein complex</v>
       </c>
       <c r="I23" t="s">
         <v>11</v>
@@ -1363,7 +1363,7 @@
         <v>$prefix-$chain-i-locus chain</v>
       </c>
       <c r="L23" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="24" spans="1:14">
@@ -1374,23 +1374,23 @@
         <v>3</v>
       </c>
       <c r="C24" t="s">
-        <v>41</v>
+        <v>74</v>
       </c>
       <c r="D24" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="E24" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="F24" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="G24" t="s">
         <v>18</v>
       </c>
       <c r="H24" t="str">
         <f>C21</f>
-        <v>$class molecule</v>
+        <v>$class protein complex</v>
       </c>
       <c r="I24" t="s">
         <v>11</v>
@@ -1412,23 +1412,23 @@
         <v>3</v>
       </c>
       <c r="C25" t="s">
-        <v>46</v>
+        <v>75</v>
       </c>
       <c r="D25" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="E25" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="F25" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="G25" t="s">
         <v>18</v>
       </c>
       <c r="H25" t="str">
         <f>C21</f>
-        <v>$class molecule</v>
+        <v>$class protein complex</v>
       </c>
       <c r="I25" t="s">
         <v>11</v>
@@ -1450,20 +1450,20 @@
         <v>4</v>
       </c>
       <c r="C26" t="s">
-        <v>47</v>
+        <v>84</v>
       </c>
       <c r="D26" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="E26" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="G26" t="s">
         <v>18</v>
       </c>
       <c r="H26" t="str">
         <f>C21</f>
-        <v>$class molecule</v>
+        <v>$class protein complex</v>
       </c>
       <c r="I26" t="s">
         <v>11</v>
@@ -1487,13 +1487,13 @@
     </row>
     <row r="27" spans="1:14">
       <c r="A27" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B27">
         <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>52</v>
+        <v>76</v>
       </c>
       <c r="D27" t="s">
         <v>11</v>
@@ -1502,7 +1502,7 @@
         <v>18</v>
       </c>
       <c r="H27" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="I27" t="s">
         <v>11</v>
@@ -1513,25 +1513,25 @@
     </row>
     <row r="28" spans="1:14">
       <c r="A28" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B28">
         <v>2</v>
       </c>
       <c r="C28" t="s">
-        <v>53</v>
+        <v>77</v>
       </c>
       <c r="D28" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="E28" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="G28" t="s">
         <v>18</v>
       </c>
       <c r="H28" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="I28" t="s">
         <v>11</v>
@@ -1543,22 +1543,22 @@
     </row>
     <row r="29" spans="1:14">
       <c r="A29" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="B29">
         <v>1</v>
       </c>
       <c r="C29" t="s">
-        <v>54</v>
+        <v>78</v>
       </c>
       <c r="D29" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="G29" t="s">
         <v>18</v>
       </c>
       <c r="H29" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="N29" t="str">
         <f>C10</f>
@@ -1567,13 +1567,13 @@
     </row>
     <row r="30" spans="1:14">
       <c r="A30" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="B30">
         <v>2</v>
       </c>
       <c r="C30" t="s">
-        <v>55</v>
+        <v>79</v>
       </c>
       <c r="D30" t="s">
         <v>11</v>
@@ -1582,7 +1582,7 @@
         <v>18</v>
       </c>
       <c r="H30" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="I30" t="s">
         <v>11</v>
@@ -1594,25 +1594,25 @@
     </row>
     <row r="31" spans="1:14">
       <c r="A31" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="B31">
         <v>3</v>
       </c>
       <c r="C31" t="s">
+        <v>80</v>
+      </c>
+      <c r="D31" t="s">
         <v>56</v>
       </c>
-      <c r="D31" t="s">
-        <v>70</v>
-      </c>
       <c r="E31" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="G31" t="s">
         <v>18</v>
       </c>
       <c r="H31" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="I31" t="s">
         <v>11</v>
@@ -1624,33 +1624,33 @@
     </row>
     <row r="32" spans="1:14">
       <c r="A32" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="B32">
         <v>1</v>
       </c>
       <c r="C32" t="s">
-        <v>58</v>
+        <v>81</v>
       </c>
       <c r="D32" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="G32" t="s">
         <v>8</v>
       </c>
       <c r="H32" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
     </row>
     <row r="33" spans="1:15">
       <c r="A33" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="B33">
         <v>2</v>
       </c>
       <c r="C33" t="s">
-        <v>59</v>
+        <v>82</v>
       </c>
       <c r="D33" t="s">
         <v>11</v>
@@ -1660,34 +1660,34 @@
       </c>
       <c r="H33" t="str">
         <f>C32</f>
-        <v>mutant $class molecule</v>
+        <v>mutant $class protein complex</v>
       </c>
     </row>
     <row r="34" spans="1:15">
       <c r="A34" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="B34">
         <v>3</v>
       </c>
       <c r="C34" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="D34" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="E34" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="G34" t="s">
         <v>8</v>
       </c>
       <c r="H34" t="str">
         <f>C33</f>
-        <v>mutant $taxon-label $class molecule</v>
+        <v>mutant $taxon-label $class protein complex</v>
       </c>
       <c r="O34" t="s">
-        <v>47</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>